<commit_message>
Final code from MD
</commit_message>
<xml_diff>
--- a/Assigment-Q4.xlsx
+++ b/Assigment-Q4.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammedj\Documents\Personnel\IITK\eMaster\Course\CS973 - Machine Learning for Cyber Security\Project\asset-v1_EMIITK+CS973-Q2+2025+type@asset+block@assn1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\githubWorkSpace\CS973\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA8B25D-1CF8-43D9-8989-73BEF575C198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF99D156-AE71-4A14-BAFD-45660FD195E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="795" windowWidth="29040" windowHeight="18240" xr2:uid="{0D76DE18-083C-4777-A214-E9F182735A94}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{0D76DE18-083C-4777-A214-E9F182735A94}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
+    <sheet name="Analysis" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="2024-10-26" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="60">
   <si>
     <t>Loss Hyperparameter</t>
   </si>
@@ -138,12 +140,90 @@
   <si>
     <t>high(tol=1e1)</t>
   </si>
+  <si>
+    <t>hinge</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> clf=LogisticRegression( max_iter=10000, solver='newton-cg', penalty='l2',  tol=1e-2, C=26)</t>
+  </si>
+  <si>
+    <t>2.443546901399986 7.061607341600029 88156.0 0.9321249999999999</t>
+  </si>
+  <si>
+    <t>Hyperparameters</t>
+  </si>
+  <si>
+    <t>Train Time (s)</t>
+  </si>
+  <si>
+    <t>Test Time (s)</t>
+  </si>
+  <si>
+    <t>Model Size (bytes)</t>
+  </si>
+  <si>
+    <t>Accuracy (%)</t>
+  </si>
+  <si>
+    <t>C=0.01, solver='newton-cg'</t>
+  </si>
+  <si>
+    <t>C=1, solver='newton-cg'</t>
+  </si>
+  <si>
+    <t>C=10, solver='newton-cg'</t>
+  </si>
+  <si>
+    <t>C=11, solver='newton-cg'</t>
+  </si>
+  <si>
+    <t>C=20, solver='newton-cg'</t>
+  </si>
+  <si>
+    <t>C=40, solver='newton-cg'</t>
+  </si>
+  <si>
+    <t>C=60, solver='newton-cg'</t>
+  </si>
+  <si>
+    <t>C=100, solver='newton-cg'</t>
+  </si>
+  <si>
+    <t>C=10, solver='newton-cg', tol=1e-10</t>
+  </si>
+  <si>
+    <t>C=11, solver='newton-cg', tol=1e-10</t>
+  </si>
+  <si>
+    <t>C=11, solver='newton-cg', tol=1e-4</t>
+  </si>
+  <si>
+    <t>C=11, solver='newton-cg', tol=1e-1</t>
+  </si>
+  <si>
+    <t>C=11, solver='newton-cg', tol=1e-4, penalty='l2'</t>
+  </si>
+  <si>
+    <t>C=11, solver='liblinear', tol=1e-4, penalty='l2'</t>
+  </si>
+  <si>
+    <t>C=11, solver='liblinear', tol=1e-4, penalty='l1'</t>
+  </si>
+  <si>
+    <t>C=11, solver='liblinear', tol=1e-10, penalty='l2'</t>
+  </si>
+  <si>
+    <t>C=40, solver='liblinear', tol=1e-4, penalty='l2'</t>
+  </si>
+  <si>
+    <t>C=1, solver='liblinear', tol=1e-4, penalty='l2'</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,8 +239,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +261,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -218,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -234,6 +325,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -385,7 +506,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet1 (2)'!$C$5</c:f>
+              <c:f>Analysis!$C$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -460,7 +581,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sheet1 (2)'!$D$4:$E$4</c:f>
+              <c:f>Analysis!$D$4:$E$4</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -474,7 +595,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet1 (2)'!$D$5:$E$5</c:f>
+              <c:f>Analysis!$D$5:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -498,7 +619,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet1 (2)'!$C$6</c:f>
+              <c:f>Analysis!$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -573,7 +694,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sheet1 (2)'!$D$4:$E$4</c:f>
+              <c:f>Analysis!$D$4:$E$4</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -587,7 +708,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet1 (2)'!$D$6:$E$6</c:f>
+              <c:f>Analysis!$D$6:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -879,7 +1000,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet1 (2)'!$C$13</c:f>
+              <c:f>Analysis!$C$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -954,7 +1075,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Sheet1 (2)'!$D$11:$G$12</c:f>
+              <c:f>Analysis!$D$11:$G$12</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -984,7 +1105,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet1 (2)'!$D$13:$G$13</c:f>
+              <c:f>Analysis!$D$13:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1014,7 +1135,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet1 (2)'!$C$14</c:f>
+              <c:f>Analysis!$C$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1089,7 +1210,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Sheet1 (2)'!$D$11:$G$12</c:f>
+              <c:f>Analysis!$D$11:$G$12</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -1119,7 +1240,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet1 (2)'!$D$14:$G$14</c:f>
+              <c:f>Analysis!$D$14:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1149,7 +1270,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet1 (2)'!$C$15</c:f>
+              <c:f>Analysis!$C$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1224,7 +1345,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Sheet1 (2)'!$D$11:$G$12</c:f>
+              <c:f>Analysis!$D$11:$G$12</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -1254,7 +1375,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet1 (2)'!$D$15:$G$15</c:f>
+              <c:f>Analysis!$D$15:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2034,6 +2155,1239 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>4.a) Linearsvc</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> With Loss hyperparameter</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14873185795595772"/>
+          <c:y val="3.7037037037037035E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2024-10-26'!$C$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>hinge</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2024-10-26'!$D$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Training Time</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2024-10-26'!$D$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>7.86</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>93.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6AE3-450D-986B-29009E8DEFAA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2024-10-26'!$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>squared hinge</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2024-10-26'!$D$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Training Time</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2024-10-26'!$D$6:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.0449999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>94.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6AE3-450D-986B-29009E8DEFAA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="79"/>
+        <c:shape val="box"/>
+        <c:axId val="581281224"/>
+        <c:axId val="581281880"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="581281224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="581281880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="581281880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="581281224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>4.b) Linear SVC vs Logistic Regression (w.r.t</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> C hyperparameter</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2024-10-26'!$C$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Low(c=0.01)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'2024-10-26'!$D$11:$G$12</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>LinearSVC</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Logistic Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>LinearSVC</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Logistic Regression</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Tranining Time</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Accuracy</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2024-10-26'!$D$13:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.39</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8804-48DC-A2B9-3E16428ADA5D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2024-10-26'!$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>medium(c=1)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'2024-10-26'!$D$11:$G$12</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>LinearSVC</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Logistic Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>LinearSVC</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Logistic Regression</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Tranining Time</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Accuracy</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2024-10-26'!$D$14:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.98851</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>94.74</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8804-48DC-A2B9-3E16428ADA5D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2024-10-26'!$C$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>high(c=10)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'2024-10-26'!$D$11:$G$12</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>LinearSVC</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Logistic Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>LinearSVC</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Logistic Regression</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Tranining Time</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Accuracy</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2024-10-26'!$D$15:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.2766</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>94.45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8804-48DC-A2B9-3E16428ADA5D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="79"/>
+        <c:overlap val="100"/>
+        <c:axId val="577133376"/>
+        <c:axId val="577133704"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="577133376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="577133704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="577133704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="577133376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2151,6 +3505,83 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="310">
   <cs:axisTitle>
@@ -3255,6 +4686,1042 @@
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:defRPr sz="800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="310">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="298">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -3817,6 +6284,87 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>361949</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EF05733-613C-4E25-BCE7-5D0B1FB44280}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C217877-04A3-43FF-904C-2EDB72EC59E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4124,11 +6672,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F027933-4716-422E-8E12-2C35CFBB4136}">
   <dimension ref="C3:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
@@ -4138,14 +6686,14 @@
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:8">
       <c r="C3" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:8">
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
@@ -4156,7 +6704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8">
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
@@ -4167,7 +6715,7 @@
         <v>94.45</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8">
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
@@ -4178,7 +6726,7 @@
         <v>94.75</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:8">
       <c r="C10" s="7" t="s">
         <v>11</v>
       </c>
@@ -4188,7 +6736,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:8">
       <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
@@ -4201,7 +6749,7 @@
       </c>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:8">
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>8</v>
@@ -4216,7 +6764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:8">
       <c r="C13" s="1" t="s">
         <v>28</v>
       </c>
@@ -4233,7 +6781,7 @@
         <v>92.25</v>
       </c>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:8">
       <c r="C14" s="1" t="s">
         <v>29</v>
       </c>
@@ -4250,7 +6798,7 @@
         <v>96.58</v>
       </c>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:8">
       <c r="C15" s="1" t="s">
         <v>30</v>
       </c>
@@ -4267,7 +6815,7 @@
         <v>96.21</v>
       </c>
     </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:17">
       <c r="C18" s="7" t="s">
         <v>13</v>
       </c>
@@ -4277,7 +6825,7 @@
       <c r="G18" s="7"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:17">
       <c r="C19" s="2" t="s">
         <v>13</v>
       </c>
@@ -4290,7 +6838,7 @@
       </c>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:17">
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>8</v>
@@ -4305,7 +6853,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:17">
       <c r="C21" s="1" t="s">
         <v>31</v>
       </c>
@@ -4318,7 +6866,7 @@
       </c>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:17">
       <c r="C22" s="1" t="s">
         <v>32</v>
       </c>
@@ -4331,7 +6879,7 @@
       </c>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:17">
       <c r="C23" s="1" t="s">
         <v>33</v>
       </c>
@@ -4344,15 +6892,15 @@
       </c>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:17">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="P24" s="5"/>
     </row>
-    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:17">
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:17">
       <c r="C26" s="7" t="s">
         <v>17</v>
       </c>
@@ -4362,7 +6910,7 @@
       <c r="G26" s="7"/>
       <c r="Q26" s="5"/>
     </row>
-    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:17">
       <c r="C27" s="2" t="s">
         <v>14</v>
       </c>
@@ -4376,7 +6924,7 @@
       <c r="G27" s="8"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:17">
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
         <v>8</v>
@@ -4392,7 +6940,7 @@
       </c>
       <c r="Q28" s="5"/>
     </row>
-    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:17">
       <c r="C29" s="1" t="s">
         <v>15</v>
       </c>
@@ -4405,7 +6953,7 @@
       </c>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:17">
       <c r="C30" s="1" t="s">
         <v>16</v>
       </c>
@@ -4445,7 +6993,7 @@
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
@@ -4455,14 +7003,14 @@
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:8">
       <c r="C3" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:8">
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
@@ -4473,7 +7021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8">
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
@@ -4484,7 +7032,7 @@
         <v>94.45</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8">
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
@@ -4495,7 +7043,7 @@
         <v>94.75</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:8">
       <c r="C10" s="7" t="s">
         <v>11</v>
       </c>
@@ -4505,7 +7053,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:8">
       <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
@@ -4521,7 +7069,7 @@
       </c>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:8">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
@@ -4537,7 +7085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:8">
       <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
@@ -4553,7 +7101,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:8">
       <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
@@ -4569,7 +7117,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:8">
       <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
@@ -4585,7 +7133,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:8">
       <c r="C18" s="7" t="s">
         <v>13</v>
       </c>
@@ -4595,7 +7143,7 @@
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:8">
       <c r="C19" s="2" t="s">
         <v>13</v>
       </c>
@@ -4611,7 +7159,7 @@
       </c>
       <c r="H19" s="8"/>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:8">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
@@ -4627,7 +7175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:8">
       <c r="C21" s="1" t="s">
         <v>5</v>
       </c>
@@ -4647,7 +7195,7 @@
         <v>98.23</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:8">
       <c r="C22" s="1" t="s">
         <v>6</v>
       </c>
@@ -4667,7 +7215,7 @@
         <v>62.36</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:8">
       <c r="C23" s="1" t="s">
         <v>7</v>
       </c>
@@ -4687,7 +7235,7 @@
         <v>95.26</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:8">
       <c r="D24" s="1" t="s">
         <v>27</v>
       </c>
@@ -4698,7 +7246,7 @@
         <v>94.74</v>
       </c>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:8">
       <c r="C26" s="7" t="s">
         <v>17</v>
       </c>
@@ -4707,7 +7255,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:8">
       <c r="C27" s="2" t="s">
         <v>14</v>
       </c>
@@ -4720,7 +7268,7 @@
       </c>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:8">
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
         <v>12</v>
@@ -4735,7 +7283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:8">
       <c r="C29" s="1" t="s">
         <v>15</v>
       </c>
@@ -4748,7 +7296,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:8">
       <c r="C30" s="1" t="s">
         <v>16</v>
       </c>
@@ -4778,4 +7326,675 @@
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA042A8D-85E4-4701-8391-E88E1CE92095}">
+  <dimension ref="E3:I21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="5:9" ht="45">
+      <c r="E3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="5:9" ht="38.25">
+      <c r="E4" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="15">
+        <v>2.0125000000000002</v>
+      </c>
+      <c r="G4" s="15">
+        <v>6.6996000000000002</v>
+      </c>
+      <c r="H4" s="15">
+        <v>88996</v>
+      </c>
+      <c r="I4" s="15">
+        <v>82.52</v>
+      </c>
+    </row>
+    <row r="5" spans="5:9" ht="38.25">
+      <c r="E5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="15">
+        <v>2.2023000000000001</v>
+      </c>
+      <c r="G5" s="15">
+        <v>7.2614000000000001</v>
+      </c>
+      <c r="H5" s="15">
+        <v>88156</v>
+      </c>
+      <c r="I5" s="15">
+        <v>93.91</v>
+      </c>
+    </row>
+    <row r="6" spans="5:9" ht="38.25">
+      <c r="E6" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="15">
+        <v>2.8464</v>
+      </c>
+      <c r="G6" s="15">
+        <v>6.8528000000000002</v>
+      </c>
+      <c r="H6" s="15">
+        <v>88156</v>
+      </c>
+      <c r="I6" s="15">
+        <v>94.95</v>
+      </c>
+    </row>
+    <row r="7" spans="5:9" ht="38.25">
+      <c r="E7" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="15">
+        <v>3.1303000000000001</v>
+      </c>
+      <c r="G7" s="15">
+        <v>7.0397999999999996</v>
+      </c>
+      <c r="H7" s="15">
+        <v>88156</v>
+      </c>
+      <c r="I7" s="15">
+        <v>94.96</v>
+      </c>
+    </row>
+    <row r="8" spans="5:9" ht="38.25">
+      <c r="E8" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="15">
+        <v>3.3007</v>
+      </c>
+      <c r="G8" s="15">
+        <v>6.6548999999999996</v>
+      </c>
+      <c r="H8" s="15">
+        <v>88156</v>
+      </c>
+      <c r="I8" s="15">
+        <v>94.96</v>
+      </c>
+    </row>
+    <row r="9" spans="5:9" ht="38.25">
+      <c r="E9" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="17">
+        <v>3.2008000000000001</v>
+      </c>
+      <c r="G9" s="17">
+        <v>6.6249000000000002</v>
+      </c>
+      <c r="H9" s="17">
+        <v>88156</v>
+      </c>
+      <c r="I9" s="17">
+        <v>94.99</v>
+      </c>
+    </row>
+    <row r="10" spans="5:9" ht="38.25">
+      <c r="E10" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="15">
+        <v>3.7298</v>
+      </c>
+      <c r="G10" s="15">
+        <v>6.2294</v>
+      </c>
+      <c r="H10" s="15">
+        <v>88156</v>
+      </c>
+      <c r="I10" s="15">
+        <v>94.96</v>
+      </c>
+    </row>
+    <row r="11" spans="5:9" ht="38.25">
+      <c r="E11" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="15">
+        <v>3.4016000000000002</v>
+      </c>
+      <c r="G11" s="15">
+        <v>6.7072000000000003</v>
+      </c>
+      <c r="H11" s="15">
+        <v>88156</v>
+      </c>
+      <c r="I11" s="15">
+        <v>94.93</v>
+      </c>
+    </row>
+    <row r="12" spans="5:9" ht="51">
+      <c r="E12" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="15">
+        <v>4.2392000000000003</v>
+      </c>
+      <c r="G12" s="15">
+        <v>6.4560000000000004</v>
+      </c>
+      <c r="H12" s="15">
+        <v>88156</v>
+      </c>
+      <c r="I12" s="15">
+        <v>94.95</v>
+      </c>
+    </row>
+    <row r="13" spans="5:9" ht="51">
+      <c r="E13" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="15">
+        <v>3.8138000000000001</v>
+      </c>
+      <c r="G13" s="15">
+        <v>7.0993000000000004</v>
+      </c>
+      <c r="H13" s="15">
+        <v>88156</v>
+      </c>
+      <c r="I13" s="15">
+        <v>94.96</v>
+      </c>
+    </row>
+    <row r="14" spans="5:9" ht="51">
+      <c r="E14" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="15">
+        <v>2.1305000000000001</v>
+      </c>
+      <c r="G14" s="15">
+        <v>7.4913999999999996</v>
+      </c>
+      <c r="H14" s="15">
+        <v>88156</v>
+      </c>
+      <c r="I14" s="15">
+        <v>94.96</v>
+      </c>
+    </row>
+    <row r="15" spans="5:9" ht="51">
+      <c r="E15" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="15">
+        <v>1.0447</v>
+      </c>
+      <c r="G15" s="15">
+        <v>7.0262000000000002</v>
+      </c>
+      <c r="H15" s="15">
+        <v>88156</v>
+      </c>
+      <c r="I15" s="15">
+        <v>79.06</v>
+      </c>
+    </row>
+    <row r="16" spans="5:9" ht="76.5">
+      <c r="E16" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="15">
+        <v>3.1452</v>
+      </c>
+      <c r="G16" s="15">
+        <v>6.4869000000000003</v>
+      </c>
+      <c r="H16" s="15">
+        <v>88156</v>
+      </c>
+      <c r="I16" s="15">
+        <v>94.96</v>
+      </c>
+    </row>
+    <row r="17" spans="5:9" ht="76.5">
+      <c r="E17" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="19">
+        <v>0.99150000000000005</v>
+      </c>
+      <c r="G17" s="19">
+        <v>7.0486000000000004</v>
+      </c>
+      <c r="H17" s="19">
+        <v>88156</v>
+      </c>
+      <c r="I17" s="19">
+        <v>94.88</v>
+      </c>
+    </row>
+    <row r="18" spans="5:9" ht="76.5">
+      <c r="E18" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="15">
+        <v>3.7357</v>
+      </c>
+      <c r="G18" s="15">
+        <v>6.4123000000000001</v>
+      </c>
+      <c r="H18" s="15">
+        <v>88156</v>
+      </c>
+      <c r="I18" s="15">
+        <v>94.77</v>
+      </c>
+    </row>
+    <row r="19" spans="5:9" ht="89.25">
+      <c r="E19" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="15">
+        <v>1.1686000000000001</v>
+      </c>
+      <c r="G19" s="15">
+        <v>7.2849000000000004</v>
+      </c>
+      <c r="H19" s="15">
+        <v>88156</v>
+      </c>
+      <c r="I19" s="15">
+        <v>94.87</v>
+      </c>
+    </row>
+    <row r="20" spans="5:9" ht="76.5">
+      <c r="E20" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="15">
+        <v>1.5101</v>
+      </c>
+      <c r="G20" s="15">
+        <v>6.7427000000000001</v>
+      </c>
+      <c r="H20" s="15">
+        <v>88156</v>
+      </c>
+      <c r="I20" s="15">
+        <v>94.95</v>
+      </c>
+    </row>
+    <row r="21" spans="5:9" ht="76.5">
+      <c r="E21" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" s="11">
+        <v>0.78369999999999995</v>
+      </c>
+      <c r="G21" s="11">
+        <v>7.3452999999999999</v>
+      </c>
+      <c r="H21" s="11">
+        <v>88156</v>
+      </c>
+      <c r="I21" s="11">
+        <v>94.04</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDBAD5E8-728B-4EEE-8403-3077F3F0CE12}">
+  <dimension ref="C3:Q33"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:8">
+      <c r="C3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="3:8">
+      <c r="C4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8">
+      <c r="C5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="1">
+        <v>7.86</v>
+      </c>
+      <c r="E5" s="1">
+        <v>93.98</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8">
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.0449999999999999</v>
+      </c>
+      <c r="E6" s="1">
+        <v>94.75</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8">
+      <c r="C10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="3:8">
+      <c r="C11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="3:8">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8">
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1.0329999999999999</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1">
+        <v>90.39</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="3:8">
+      <c r="C14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.98851</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1">
+        <v>94.74</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="3:8">
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1.2766</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1">
+        <v>94.45</v>
+      </c>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="18" spans="3:17">
+      <c r="C18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="3:17">
+      <c r="C19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="3:17">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="3:17">
+      <c r="C21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1.0680000000000001</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1">
+        <v>94.74</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="3:17">
+      <c r="C22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1.139</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1">
+        <v>94.74</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="3:17">
+      <c r="C23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.85209999999999997</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1">
+        <v>61.71</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="3:17">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="P24" s="5"/>
+    </row>
+    <row r="25" spans="3:17">
+      <c r="Q25" s="5"/>
+    </row>
+    <row r="26" spans="3:17">
+      <c r="C26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="Q26" s="5"/>
+    </row>
+    <row r="27" spans="3:17">
+      <c r="C27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" s="8"/>
+      <c r="Q27" s="5"/>
+    </row>
+    <row r="28" spans="3:17">
+      <c r="C28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q28" s="5"/>
+    </row>
+    <row r="29" spans="3:17">
+      <c r="C29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="1">
+        <v>11.29</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1">
+        <v>94.59</v>
+      </c>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="3:17">
+      <c r="C30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1.3242</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1">
+        <v>94.75</v>
+      </c>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="32" spans="3:17">
+      <c r="C32" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+    </row>
+    <row r="33" spans="3:7">
+      <c r="C33" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>